<commit_message>
added sample type check to checklist
</commit_message>
<xml_diff>
--- a/inst/rmarkdown/templates/visc_report/skeleton/Checklist_PT_Report.xlsx
+++ b/inst/rmarkdown/templates/visc_report/skeleton/Checklist_PT_Report.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projects\scharpTemplates\inst\rmarkdown\templates\visc_report\skeleton\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>PT Report Checklist</t>
   </si>
@@ -149,11 +154,14 @@
   <si>
     <t>Once completed have you committed and pushed all relevant files for the report (i.e. bib file, …)? Can someone else compile this if they cloned the repo?</t>
   </si>
+  <si>
+    <t>Is the sample type accurate (e.g., serum, plasma, PBMC)? If unsure, confirm with Michelle/Eva.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,6 +232,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -325,6 +336,10 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -380,7 +395,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -388,6 +403,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -421,7 +459,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -429,6 +467,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -462,7 +523,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -470,6 +531,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -503,7 +587,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -511,6 +595,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -544,7 +651,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -552,6 +659,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -585,7 +715,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -593,6 +723,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -626,7 +779,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -634,6 +787,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -667,7 +843,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -675,6 +851,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -708,7 +907,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -716,6 +915,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -749,7 +971,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -757,6 +979,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -790,7 +1035,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -798,6 +1043,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -831,7 +1099,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -839,6 +1107,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -872,7 +1163,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -880,6 +1171,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -913,7 +1227,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -921,6 +1235,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -954,7 +1291,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -962,6 +1299,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -995,7 +1355,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1003,6 +1363,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1036,7 +1419,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1044,6 +1427,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1077,7 +1483,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1085,6 +1491,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1118,7 +1547,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1126,6 +1555,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1159,7 +1611,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1167,6 +1619,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1200,7 +1675,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1208,6 +1683,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1221,13 +1719,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>53</xdr:row>
+          <xdr:row>54</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>53</xdr:row>
+          <xdr:row>54</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1241,7 +1739,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1249,6 +1747,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1262,13 +1783,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>52</xdr:row>
+          <xdr:row>53</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>52</xdr:row>
+          <xdr:row>53</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1282,7 +1803,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1290,6 +1811,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1303,13 +1847,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>51</xdr:row>
+          <xdr:row>52</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>51</xdr:row>
+          <xdr:row>52</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1323,7 +1867,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1331,6 +1875,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1344,13 +1911,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>50</xdr:row>
+          <xdr:row>51</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>50</xdr:row>
+          <xdr:row>51</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1364,7 +1931,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1372,6 +1939,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1385,13 +1975,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>49</xdr:row>
+          <xdr:row>50</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>49</xdr:row>
+          <xdr:row>50</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1405,7 +1995,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1413,6 +2003,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1426,13 +2039,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>57</xdr:row>
+          <xdr:row>58</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>57</xdr:row>
+          <xdr:row>58</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1446,7 +2059,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1454,6 +2067,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1467,13 +2103,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>65</xdr:row>
+          <xdr:row>66</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>65</xdr:row>
+          <xdr:row>66</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1487,7 +2123,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1495,6 +2131,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1508,13 +2167,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>66</xdr:row>
+          <xdr:row>67</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>66</xdr:row>
+          <xdr:row>67</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1528,7 +2187,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1536,6 +2195,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1549,13 +2231,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>67</xdr:row>
+          <xdr:row>68</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>67</xdr:row>
+          <xdr:row>68</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1569,7 +2251,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1577,6 +2259,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1590,13 +2295,13 @@
         <xdr:from>
           <xdr:col>0</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>61</xdr:row>
+          <xdr:row>62</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>61</xdr:row>
+          <xdr:row>62</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -1610,7 +2315,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1618,10 +2323,92 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
       </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>76200</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="295275" cy="190500"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1066" name="Check Box 42" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1066"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -1671,7 +2458,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1706,7 +2493,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1915,10 +2702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2136,102 +2923,108 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B49" s="2"/>
+    <row r="49" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B55" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B57" s="2"/>
-    </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B59" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B62" s="2" t="s">
+    <row r="62" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B63" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B66" s="2" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B67" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B67" s="2" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B68" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B68" s="2" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B69" s="2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1026" r:id="rId3" name="Check Box 2">
+            <control shapeId="1026" r:id="rId4" name="Check Box 2">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2253,7 +3046,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1036" r:id="rId4" name="Check Box 12">
+            <control shapeId="1036" r:id="rId5" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2275,7 +3068,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1037" r:id="rId5" name="Check Box 13">
+            <control shapeId="1037" r:id="rId6" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2297,7 +3090,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1038" r:id="rId6" name="Check Box 14">
+            <control shapeId="1038" r:id="rId7" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2319,7 +3112,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1039" r:id="rId7" name="Check Box 15">
+            <control shapeId="1039" r:id="rId8" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2341,7 +3134,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1040" r:id="rId8" name="Check Box 16">
+            <control shapeId="1040" r:id="rId9" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2363,7 +3156,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1041" r:id="rId9" name="Check Box 17">
+            <control shapeId="1041" r:id="rId10" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2385,7 +3178,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1042" r:id="rId10" name="Check Box 18">
+            <control shapeId="1042" r:id="rId11" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2407,7 +3200,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1043" r:id="rId11" name="Check Box 19">
+            <control shapeId="1043" r:id="rId12" name="Check Box 19">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2429,7 +3222,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1044" r:id="rId12" name="Check Box 20">
+            <control shapeId="1044" r:id="rId13" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2451,7 +3244,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1045" r:id="rId13" name="Check Box 21">
+            <control shapeId="1045" r:id="rId14" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2473,7 +3266,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId14" name="Check Box 22">
+            <control shapeId="1046" r:id="rId15" name="Check Box 22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2495,7 +3288,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1047" r:id="rId15" name="Check Box 23">
+            <control shapeId="1047" r:id="rId16" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2517,7 +3310,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId16" name="Check Box 24">
+            <control shapeId="1048" r:id="rId17" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2539,7 +3332,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1049" r:id="rId17" name="Check Box 25">
+            <control shapeId="1049" r:id="rId18" name="Check Box 25">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2561,7 +3354,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId18" name="Check Box 26">
+            <control shapeId="1050" r:id="rId19" name="Check Box 26">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2583,7 +3376,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1051" r:id="rId19" name="Check Box 27">
+            <control shapeId="1051" r:id="rId20" name="Check Box 27">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2605,7 +3398,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1052" r:id="rId20" name="Check Box 28">
+            <control shapeId="1052" r:id="rId21" name="Check Box 28">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2627,7 +3420,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1053" r:id="rId21" name="Check Box 29">
+            <control shapeId="1053" r:id="rId22" name="Check Box 29">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2649,7 +3442,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1054" r:id="rId22" name="Check Box 30">
+            <control shapeId="1054" r:id="rId23" name="Check Box 30">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2671,7 +3464,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1055" r:id="rId23" name="Check Box 31">
+            <control shapeId="1055" r:id="rId24" name="Check Box 31">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2693,7 +3486,29 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1056" r:id="rId24" name="Check Box 32">
+            <control shapeId="1056" r:id="rId25" name="Check Box 32">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>54</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>371475</xdr:colOff>
+                    <xdr:row>54</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1057" r:id="rId26" name="Check Box 33">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2715,7 +3530,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1057" r:id="rId25" name="Check Box 33">
+            <control shapeId="1058" r:id="rId27" name="Check Box 34">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2737,7 +3552,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1058" r:id="rId26" name="Check Box 34">
+            <control shapeId="1059" r:id="rId28" name="Check Box 35">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2759,7 +3574,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1059" r:id="rId27" name="Check Box 35">
+            <control shapeId="1060" r:id="rId29" name="Check Box 36">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2781,19 +3596,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1060" r:id="rId28" name="Check Box 36">
+            <control shapeId="1061" r:id="rId30" name="Check Box 37">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>49</xdr:row>
+                    <xdr:row>58</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>49</xdr:row>
+                    <xdr:row>58</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
                 </anchor>
@@ -2803,51 +3618,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1061" r:id="rId29" name="Check Box 37">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>57</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>57</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1062" r:id="rId30" name="Check Box 38">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>65</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>65</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1063" r:id="rId31" name="Check Box 39">
+            <control shapeId="1062" r:id="rId31" name="Check Box 38">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2869,7 +3640,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1064" r:id="rId32" name="Check Box 40">
+            <control shapeId="1063" r:id="rId32" name="Check Box 39">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -2891,19 +3662,63 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1065" r:id="rId33" name="Check Box 41">
+            <control shapeId="1064" r:id="rId33" name="Check Box 40">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>61</xdr:row>
+                    <xdr:row>68</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
                     <xdr:colOff>371475</xdr:colOff>
-                    <xdr:row>61</xdr:row>
+                    <xdr:row>68</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1065" r:id="rId34" name="Check Box 41">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>62</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>371475</xdr:colOff>
+                    <xdr:row>62</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1066" r:id="rId35" name="Check Box 42">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>76200</xdr:colOff>
+                    <xdr:row>49</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>371475</xdr:colOff>
+                    <xdr:row>49</xdr:row>
                     <xdr:rowOff>209550</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>